<commit_message>
changed language and color scheme for simulation visualization
</commit_message>
<xml_diff>
--- a/assets/data/Perimetro_Prev/Data_Riesgo_MANUAL_Perimetro_Prev.xlsx
+++ b/assets/data/Perimetro_Prev/Data_Riesgo_MANUAL_Perimetro_Prev.xlsx
@@ -13761,7 +13761,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -14016,7 +14016,7 @@
         <v>3</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">

</xml_diff>